<commit_message>
Add support for "Format only cells that contain" using a formula.
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -471,7 +471,125 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -777,7 +895,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,13 +982,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>($A$1=A2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,6 +1042,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -20061,35 +20208,26 @@
 </easyPacket>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>